<commit_message>
Saving the tracker - I believe this will be redundant because of the migration to google sheets
</commit_message>
<xml_diff>
--- a/leetcode/tracker.xlsx
+++ b/leetcode/tracker.xlsx
@@ -5,16 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\OneDrive - ARK\programs\code\leetcode\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://agnesh-my.sharepoint.com/personal/agnesh_agnesh_onmicrosoft_com/Documents/programs/code/leetcode/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E27BF67-A647-45FD-B8E5-A4B189523DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="6_{9EEEB6E0-D705-456C-AD27-F14934ED38E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F85847AB-07D4-4E86-A851-AD6B62C63539}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leet" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">leet!$H$1:$H$65</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="191">
   <si>
     <t>Two Sum - LeetCode</t>
   </si>
@@ -574,6 +578,30 @@
   </si>
   <si>
     <t>Insert numbers into a set, then start a sequence only at numbers without a predecessor and expand to find the longest streak.</t>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/description/</t>
+  </si>
+  <si>
+    <t>Sum of Two Integers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-of-two-integers/description/</t>
+  </si>
+  <si>
+    <t>Number of 1 Bits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-1-bits/description/</t>
+  </si>
+  <si>
+    <t>Counting Bits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/counting-bits/description/</t>
   </si>
 </sst>
 </file>
@@ -684,11 +712,74 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -724,6 +815,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,27 +1086,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC9C734-1856-40B5-B14B-DBBAFE9DC413}">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="150" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="101.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1"/>
-    <col min="9" max="9" width="8.85546875" style="4"/>
-    <col min="10" max="10" width="19.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="80.85546875" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="31.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="101.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="8.88671875" style="4"/>
+    <col min="10" max="10" width="19.88671875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="80.88671875" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>157</v>
       </c>
@@ -1046,7 +1141,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="6" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="1">
         <v>1</v>
@@ -1076,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>45530</v>
       </c>
@@ -1111,7 +1206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45505</v>
       </c>
@@ -1143,7 +1238,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>11</v>
       </c>
@@ -1172,7 +1267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>15</v>
       </c>
@@ -1198,7 +1293,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>19</v>
       </c>
@@ -1227,7 +1322,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>20</v>
       </c>
@@ -1256,7 +1351,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>21</v>
       </c>
@@ -1285,7 +1380,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>46</v>
       </c>
@@ -1305,7 +1400,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>45558</v>
       </c>
@@ -1340,421 +1435,395 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>45510</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>70</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>25</v>
+        <v>148</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>100</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="F15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="H15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K15" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
         <v>102</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="F16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K16" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
         <v>104</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>45496</v>
-      </c>
-      <c r="B17" s="1">
-        <v>121</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J17" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="K17" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>45531</v>
+        <v>45496</v>
       </c>
       <c r="B18" s="1">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>45531</v>
+      </c>
+      <c r="B19" s="1">
+        <v>125</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="F19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="4" t="s">
+      <c r="H19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>45505</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>128</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="F20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="4" t="s">
+      <c r="H20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K20" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>45500</v>
-      </c>
-      <c r="B20" s="1">
-        <v>141</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>45500</v>
       </c>
       <c r="B21" s="1">
+        <v>141</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>45500</v>
+      </c>
+      <c r="B22" s="1">
         <v>142</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="F22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="2" t="s">
+      <c r="H22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K22" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
         <v>147</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K23" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
         <v>167</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="F24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K24" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>45512</v>
-      </c>
-      <c r="B24" s="1">
-        <v>198</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>45512</v>
       </c>
       <c r="B26" s="1">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
@@ -1763,260 +1832,254 @@
         <v>147</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>91</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>83</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>91</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>45512</v>
+      </c>
       <c r="B28" s="1">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D28" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="E28" s="2" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>46</v>
+        <v>153</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D29" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="E29" s="2" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>45503</v>
-      </c>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>45500</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>45503</v>
       </c>
       <c r="B32" s="1">
-        <v>271</v>
+        <v>238</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>45500</v>
+      </c>
+      <c r="B33" s="1">
+        <v>242</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>45503</v>
+      </c>
+      <c r="B34" s="1">
+        <v>271</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2" t="s">
+      <c r="F34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K32" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>45514</v>
-      </c>
-      <c r="B33" s="1">
-        <v>300</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>45515</v>
-      </c>
-      <c r="B34" s="1">
-        <v>322</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>91</v>
@@ -2025,71 +2088,68 @@
         <v>18</v>
       </c>
       <c r="J34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>45514</v>
+      </c>
+      <c r="B35" s="1">
+        <v>300</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K34" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>45569</v>
-      </c>
-      <c r="B35" s="1">
-        <v>347</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K35" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>45510</v>
+        <v>45515</v>
       </c>
       <c r="B36" s="1">
-        <v>424</v>
+        <v>322</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>91</v>
@@ -2098,315 +2158,422 @@
         <v>18</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>45492</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
-        <v>572</v>
+        <v>338</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>45569</v>
+      </c>
+      <c r="B38" s="1">
+        <v>347</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
+        <v>371</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>45510</v>
+      </c>
+      <c r="B40" s="1">
+        <v>424</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>45492</v>
+      </c>
+      <c r="B41" s="1">
+        <v>572</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J37" s="2" t="s">
+      <c r="H41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K37" s="8" t="s">
+      <c r="K41" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="1">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
         <v>876</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G38" s="2" t="s">
+      <c r="F42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J42" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K38" s="8" t="s">
+      <c r="K42" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+    <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
         <v>45515</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B43" s="1">
         <v>1143</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I39" s="4" t="s">
+      <c r="H43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I43" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="K39" s="10" t="s">
+      <c r="K43" s="10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="1">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B44" s="1">
         <v>1190</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="C44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K40" s="8" t="s">
+      <c r="K44" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="1">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B45" s="1">
         <v>1701</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="C45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="F45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K41" s="8" t="s">
+      <c r="K45" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+    <row r="46" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
         <v>45497</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B46" s="1">
         <v>2191</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="C46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J46" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K42" s="8" t="s">
+      <c r="K46" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="1" t="s">
+    <row r="47" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C49" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="1" t="s">
+      <c r="H49" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C50" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D45" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D46" s="1" t="s">
+      <c r="H50" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D51" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D52" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D48" s="1" t="s">
+      <c r="H52" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E53" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E54" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E55" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D57" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E57" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D58" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D50" s="1" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E59" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="3"/>
+      <c r="D60" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D51" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D52" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E54" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E55" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E56" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="E60" s="2"/>
       <c r="G60" s="2"/>
       <c r="I60" s="4"/>
       <c r="J60" s="2"/>
       <c r="K60" s="7"/>
-    </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
+      <c r="C61" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E61" s="2"/>
       <c r="G61" s="2"/>
       <c r="I61" s="4"/>
       <c r="J61" s="2"/>
       <c r="K61" s="7"/>
-    </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="E62" s="2"/>
       <c r="G62" s="2"/>
@@ -2414,7 +2581,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="E63" s="2"/>
       <c r="G63" s="2"/>
@@ -2422,7 +2589,7 @@
       <c r="J63" s="2"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="E64" s="2"/>
       <c r="G64" s="2"/>
@@ -2434,15 +2601,50 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L64">
     <sortCondition ref="B1:B64"/>
   </sortState>
-  <conditionalFormatting sqref="A1:XFD64 A69:XFD69 A76:XFD1048576">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="12" priority="38">
+      <formula>$C62="Hard"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="39">
+      <formula>$C62="Medium"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="40">
+      <formula>$C62="Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62 D62:XFD62">
+    <cfRule type="expression" dxfId="9" priority="14">
+      <formula>#REF!="Hard"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="15">
+      <formula>#REF!="Medium"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="16">
+      <formula>#REF!="Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD60 C62:C64 D63:XFD64 A69:XFD69 C76:C1048576">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$C1="Hard"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$C1="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$C1="Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62 C69 D61:XFD61 D76:XFD1048576">
+    <cfRule type="expression" dxfId="3" priority="11">
+      <formula>$C62="Hard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61:XFD61 C62 C69 D76:XFD1048576">
+    <cfRule type="expression" dxfId="2" priority="12">
+      <formula>$C62="Medium"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>$C62="Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
@@ -2453,45 +2655,63 @@
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{01EB9D20-4A6D-49B6-B364-92B9759B304B}"/>
     <hyperlink ref="K5" r:id="rId2" xr:uid="{B2EAE9C6-03C0-4A98-8E5A-E1795660D63F}"/>
-    <hyperlink ref="K22" r:id="rId3" xr:uid="{66CA3E94-4252-4DDB-ACB1-A15F285D516F}"/>
+    <hyperlink ref="K23" r:id="rId3" xr:uid="{66CA3E94-4252-4DDB-ACB1-A15F285D516F}"/>
     <hyperlink ref="K10" r:id="rId4" xr:uid="{FFA66854-641C-4CBA-A32B-763441B34733}"/>
     <hyperlink ref="K7" r:id="rId5" xr:uid="{3459079A-FB1D-49D2-87A7-B0F90C94870D}"/>
-    <hyperlink ref="K28" r:id="rId6" xr:uid="{121EB419-D24B-4F42-954F-A0BB0E991292}"/>
-    <hyperlink ref="K23" r:id="rId7" xr:uid="{B332368F-36EF-441A-ABB2-615C2CFE3544}"/>
-    <hyperlink ref="K41" r:id="rId8" xr:uid="{AD05FB58-9CA8-43F1-A3EE-6776F4FA6FD1}"/>
-    <hyperlink ref="K40" r:id="rId9" xr:uid="{8899F415-00B9-413D-8147-D09376BE0810}"/>
-    <hyperlink ref="K15" r:id="rId10" xr:uid="{EAFF11E8-CA94-4C0E-B27A-B3C88CB52E9D}"/>
-    <hyperlink ref="K42" r:id="rId11" xr:uid="{10D5D78D-8D23-460A-95C3-303511165CF2}"/>
-    <hyperlink ref="K21" r:id="rId12" xr:uid="{78A3F6A8-BE53-4119-9005-BBC638CFA22C}"/>
+    <hyperlink ref="K30" r:id="rId6" xr:uid="{121EB419-D24B-4F42-954F-A0BB0E991292}"/>
+    <hyperlink ref="K24" r:id="rId7" xr:uid="{B332368F-36EF-441A-ABB2-615C2CFE3544}"/>
+    <hyperlink ref="K45" r:id="rId8" xr:uid="{AD05FB58-9CA8-43F1-A3EE-6776F4FA6FD1}"/>
+    <hyperlink ref="K44" r:id="rId9" xr:uid="{8899F415-00B9-413D-8147-D09376BE0810}"/>
+    <hyperlink ref="K16" r:id="rId10" xr:uid="{EAFF11E8-CA94-4C0E-B27A-B3C88CB52E9D}"/>
+    <hyperlink ref="K46" r:id="rId11" xr:uid="{10D5D78D-8D23-460A-95C3-303511165CF2}"/>
+    <hyperlink ref="K22" r:id="rId12" xr:uid="{78A3F6A8-BE53-4119-9005-BBC638CFA22C}"/>
     <hyperlink ref="K6" r:id="rId13" xr:uid="{718096C5-959D-4052-BB27-735FF845BE33}"/>
-    <hyperlink ref="K30" r:id="rId14" xr:uid="{3B11BBA3-BACC-4D62-AD47-25EEEFF58B8D}"/>
+    <hyperlink ref="K32" r:id="rId14" xr:uid="{3B11BBA3-BACC-4D62-AD47-25EEEFF58B8D}"/>
     <hyperlink ref="K4" r:id="rId15" xr:uid="{914468AC-D46E-4004-A8A9-B32330B8E37C}"/>
-    <hyperlink ref="K19" r:id="rId16" xr:uid="{BEC4FAA3-023D-4522-881D-C7320CF9F9DD}"/>
-    <hyperlink ref="K36" r:id="rId17" xr:uid="{CD567A6E-62A9-4EF2-AEBC-235F38D52C4F}"/>
-    <hyperlink ref="K24" r:id="rId18" xr:uid="{0F8B6ED9-62DC-420C-8E69-2B33A4CEDB39}"/>
-    <hyperlink ref="K26" r:id="rId19" xr:uid="{316F9A52-640A-4F55-8C12-2593B398C93E}"/>
-    <hyperlink ref="K33" r:id="rId20" xr:uid="{46B362F7-5854-4E8C-ACCD-589BEA05452E}"/>
+    <hyperlink ref="K20" r:id="rId16" xr:uid="{BEC4FAA3-023D-4522-881D-C7320CF9F9DD}"/>
+    <hyperlink ref="K40" r:id="rId17" xr:uid="{CD567A6E-62A9-4EF2-AEBC-235F38D52C4F}"/>
+    <hyperlink ref="K26" r:id="rId18" xr:uid="{0F8B6ED9-62DC-420C-8E69-2B33A4CEDB39}"/>
+    <hyperlink ref="K28" r:id="rId19" xr:uid="{316F9A52-640A-4F55-8C12-2593B398C93E}"/>
+    <hyperlink ref="K35" r:id="rId20" xr:uid="{46B362F7-5854-4E8C-ACCD-589BEA05452E}"/>
     <hyperlink ref="K2" r:id="rId21" display="https://leetcode.com/problems/two-sum/description/" xr:uid="{B629F431-9AFE-404A-97A5-FA10CA6205B9}"/>
-    <hyperlink ref="K13" r:id="rId22" xr:uid="{B745C861-34AA-4874-8592-D8323DDC31B1}"/>
-    <hyperlink ref="K25" r:id="rId23" xr:uid="{AA1C5D5C-8904-4618-9336-8D831BF6D288}"/>
-    <hyperlink ref="K38" r:id="rId24" xr:uid="{66719EB6-A332-4719-891C-B855BE5B1EE7}"/>
-    <hyperlink ref="K16" r:id="rId25" xr:uid="{FE992E57-BB8D-4231-89AD-9E12CDCDB6FF}"/>
-    <hyperlink ref="K29" r:id="rId26" xr:uid="{2ABFA77E-4F13-4A0B-B698-08A553279F72}"/>
+    <hyperlink ref="K14" r:id="rId22" xr:uid="{B745C861-34AA-4874-8592-D8323DDC31B1}"/>
+    <hyperlink ref="K27" r:id="rId23" xr:uid="{AA1C5D5C-8904-4618-9336-8D831BF6D288}"/>
+    <hyperlink ref="K42" r:id="rId24" xr:uid="{66719EB6-A332-4719-891C-B855BE5B1EE7}"/>
+    <hyperlink ref="K17" r:id="rId25" xr:uid="{FE992E57-BB8D-4231-89AD-9E12CDCDB6FF}"/>
+    <hyperlink ref="K31" r:id="rId26" xr:uid="{2ABFA77E-4F13-4A0B-B698-08A553279F72}"/>
     <hyperlink ref="K8" r:id="rId27" xr:uid="{7EFBEF09-106B-4C93-A2F4-C51B31C79691}"/>
     <hyperlink ref="K9" r:id="rId28" xr:uid="{2981A90D-CFDA-483B-8AE3-2DF3854EE90A}"/>
-    <hyperlink ref="K14" r:id="rId29" xr:uid="{96035529-AF25-4A6C-85E3-257D505DAE83}"/>
-    <hyperlink ref="K27" r:id="rId30" xr:uid="{D15CE4CD-6FF6-4CAF-ADE7-0F9AA3F34A27}"/>
-    <hyperlink ref="K37" r:id="rId31" xr:uid="{87A981FE-E2F6-471D-BF9F-B9726FB7C865}"/>
-    <hyperlink ref="K17" r:id="rId32" xr:uid="{E1B1DF3F-F9DA-4068-9B40-CAD754BCD6A2}"/>
-    <hyperlink ref="K31" r:id="rId33" xr:uid="{8EA5B919-E348-4B0B-A1A0-582FA80B5657}"/>
-    <hyperlink ref="K20" r:id="rId34" xr:uid="{354EBB5E-C597-4204-AD5C-62D8EF46C33E}"/>
-    <hyperlink ref="K32" r:id="rId35" xr:uid="{6ACA2667-9C31-454F-AD8F-DE49DF9D0030}"/>
-    <hyperlink ref="K12" r:id="rId36" xr:uid="{4561E427-641C-4B88-A750-2AF146B8EE17}"/>
-    <hyperlink ref="K34" r:id="rId37" xr:uid="{6CF8E004-1A8F-4591-8B30-AD3F94092F75}"/>
-    <hyperlink ref="K39" r:id="rId38" xr:uid="{6C48852D-AC16-4020-A6D5-D6D75B05A33F}"/>
+    <hyperlink ref="K15" r:id="rId29" xr:uid="{96035529-AF25-4A6C-85E3-257D505DAE83}"/>
+    <hyperlink ref="K29" r:id="rId30" xr:uid="{D15CE4CD-6FF6-4CAF-ADE7-0F9AA3F34A27}"/>
+    <hyperlink ref="K41" r:id="rId31" xr:uid="{87A981FE-E2F6-471D-BF9F-B9726FB7C865}"/>
+    <hyperlink ref="K18" r:id="rId32" xr:uid="{E1B1DF3F-F9DA-4068-9B40-CAD754BCD6A2}"/>
+    <hyperlink ref="K33" r:id="rId33" xr:uid="{8EA5B919-E348-4B0B-A1A0-582FA80B5657}"/>
+    <hyperlink ref="K21" r:id="rId34" xr:uid="{354EBB5E-C597-4204-AD5C-62D8EF46C33E}"/>
+    <hyperlink ref="K34" r:id="rId35" xr:uid="{6ACA2667-9C31-454F-AD8F-DE49DF9D0030}"/>
+    <hyperlink ref="K13" r:id="rId36" xr:uid="{4561E427-641C-4B88-A750-2AF146B8EE17}"/>
+    <hyperlink ref="K36" r:id="rId37" xr:uid="{6CF8E004-1A8F-4591-8B30-AD3F94092F75}"/>
+    <hyperlink ref="K43" r:id="rId38" xr:uid="{6C48852D-AC16-4020-A6D5-D6D75B05A33F}"/>
     <hyperlink ref="K11" r:id="rId39" xr:uid="{485E811F-CA64-4519-8113-59D6DF6108B3}"/>
+    <hyperlink ref="K12" r:id="rId40" xr:uid="{F4374F49-D10B-4344-8C82-E6E2B0C36E84}"/>
+    <hyperlink ref="K39" r:id="rId41" xr:uid="{A55CA948-D03B-4577-ADAD-8697BE4DF864}"/>
+    <hyperlink ref="K25" r:id="rId42" xr:uid="{9163830E-ACE5-4E0A-ACAE-36F9D23E7E31}"/>
+    <hyperlink ref="K37" r:id="rId43" xr:uid="{C41263C6-9891-4E37-BC33-E69CC32FF7D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A616EC-9E91-4C57-AB8A-FCDA711E7105}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" zoomScale="270" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>